<commit_message>
Final update to burndown chart
</commit_message>
<xml_diff>
--- a/agile/burndown/Team Blue Burndown Chart.xlsx
+++ b/agile/burndown/Team Blue Burndown Chart.xlsx
@@ -1661,6 +1661,18 @@
     <xf numFmtId="0" fontId="2" fillId="9" borderId="4" xfId="4" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1699,18 +1711,6 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="12" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2919,25 +2919,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>77</c:v>
+                  <c:v>79</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>65.5</c:v>
+                  <c:v>67.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>55</c:v>
+                  <c:v>57</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>42.5</c:v>
+                  <c:v>44.5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>25.5</c:v>
+                  <c:v>27.5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>18.5</c:v>
+                  <c:v>20.5</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.5</c:v>
+                  <c:v>3.5</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>0</c:v>
@@ -2985,25 +2985,25 @@
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>77</c:v>
+                  <c:v>79</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>66</c:v>
+                  <c:v>67.714285714285708</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>55</c:v>
+                  <c:v>56.428571428571423</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>44</c:v>
+                  <c:v>45.142857142857139</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>33</c:v>
+                  <c:v>33.857142857142854</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>22</c:v>
+                  <c:v>22.571428571428569</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>11</c:v>
+                  <c:v>11.285714285714283</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>0</c:v>
@@ -3636,57 +3636,57 @@
   <sheetData>
     <row r="1" spans="1:23" ht="49.8" x14ac:dyDescent="0.8">
       <c r="A1" s="24"/>
-      <c r="B1" s="87" t="s">
+      <c r="B1" s="91" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="87"/>
-      <c r="D1" s="87"/>
-      <c r="E1" s="87"/>
-      <c r="F1" s="87"/>
-      <c r="G1" s="87"/>
-      <c r="H1" s="87"/>
-      <c r="I1" s="87"/>
-      <c r="J1" s="87"/>
-      <c r="K1" s="87"/>
-      <c r="L1" s="87"/>
-      <c r="M1" s="87"/>
-      <c r="N1" s="87"/>
-      <c r="O1" s="87"/>
-      <c r="P1" s="87"/>
-      <c r="Q1" s="87"/>
-      <c r="R1" s="87"/>
-      <c r="S1" s="87"/>
-      <c r="T1" s="87"/>
-      <c r="U1" s="87"/>
-      <c r="V1" s="87"/>
-      <c r="W1" s="87"/>
+      <c r="C1" s="91"/>
+      <c r="D1" s="91"/>
+      <c r="E1" s="91"/>
+      <c r="F1" s="91"/>
+      <c r="G1" s="91"/>
+      <c r="H1" s="91"/>
+      <c r="I1" s="91"/>
+      <c r="J1" s="91"/>
+      <c r="K1" s="91"/>
+      <c r="L1" s="91"/>
+      <c r="M1" s="91"/>
+      <c r="N1" s="91"/>
+      <c r="O1" s="91"/>
+      <c r="P1" s="91"/>
+      <c r="Q1" s="91"/>
+      <c r="R1" s="91"/>
+      <c r="S1" s="91"/>
+      <c r="T1" s="91"/>
+      <c r="U1" s="91"/>
+      <c r="V1" s="91"/>
+      <c r="W1" s="91"/>
     </row>
     <row r="2" spans="1:23" ht="33" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A2" s="24"/>
-      <c r="B2" s="88" t="s">
+      <c r="B2" s="92" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="88"/>
-      <c r="D2" s="88"/>
-      <c r="E2" s="88"/>
-      <c r="F2" s="88"/>
-      <c r="G2" s="88"/>
-      <c r="H2" s="88"/>
-      <c r="I2" s="88"/>
-      <c r="J2" s="88"/>
-      <c r="K2" s="88"/>
-      <c r="L2" s="88"/>
-      <c r="M2" s="88"/>
-      <c r="N2" s="88"/>
-      <c r="O2" s="88"/>
-      <c r="P2" s="88"/>
-      <c r="Q2" s="88"/>
-      <c r="R2" s="88"/>
-      <c r="S2" s="88"/>
-      <c r="T2" s="88"/>
-      <c r="U2" s="88"/>
-      <c r="V2" s="88"/>
-      <c r="W2" s="88"/>
+      <c r="C2" s="92"/>
+      <c r="D2" s="92"/>
+      <c r="E2" s="92"/>
+      <c r="F2" s="92"/>
+      <c r="G2" s="92"/>
+      <c r="H2" s="92"/>
+      <c r="I2" s="92"/>
+      <c r="J2" s="92"/>
+      <c r="K2" s="92"/>
+      <c r="L2" s="92"/>
+      <c r="M2" s="92"/>
+      <c r="N2" s="92"/>
+      <c r="O2" s="92"/>
+      <c r="P2" s="92"/>
+      <c r="Q2" s="92"/>
+      <c r="R2" s="92"/>
+      <c r="S2" s="92"/>
+      <c r="T2" s="92"/>
+      <c r="U2" s="92"/>
+      <c r="V2" s="92"/>
+      <c r="W2" s="92"/>
     </row>
     <row r="3" spans="1:23" s="1" customFormat="1" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="22"/>
@@ -3694,20 +3694,20 @@
       <c r="C3" s="30"/>
       <c r="D3" s="30"/>
       <c r="E3" s="30"/>
-      <c r="F3" s="89" t="s">
+      <c r="F3" s="93" t="s">
         <v>31</v>
       </c>
-      <c r="G3" s="90"/>
-      <c r="H3" s="90"/>
-      <c r="I3" s="90"/>
-      <c r="J3" s="91"/>
-      <c r="K3" s="92" t="s">
+      <c r="G3" s="94"/>
+      <c r="H3" s="94"/>
+      <c r="I3" s="94"/>
+      <c r="J3" s="95"/>
+      <c r="K3" s="96" t="s">
         <v>32</v>
       </c>
-      <c r="L3" s="93"/>
-      <c r="M3" s="93"/>
-      <c r="N3" s="93"/>
-      <c r="O3" s="94"/>
+      <c r="L3" s="97"/>
+      <c r="M3" s="97"/>
+      <c r="N3" s="97"/>
+      <c r="O3" s="98"/>
       <c r="P3" s="62"/>
       <c r="Q3" s="31"/>
       <c r="R3" s="31"/>
@@ -3841,13 +3841,13 @@
         <f t="shared" ref="P6:P25" si="0">IF(D6="","-",(IF(COUNT(E6:O6) = 0,"To Do",IF(E6&gt;SUM(F6:O6),"Incomplete","Done"))))</f>
         <v>Done</v>
       </c>
-      <c r="R6" s="95" t="s">
+      <c r="R6" s="99" t="s">
         <v>4</v>
       </c>
-      <c r="S6" s="98"/>
-      <c r="T6" s="98"/>
-      <c r="U6" s="98"/>
-      <c r="V6" s="99"/>
+      <c r="S6" s="102"/>
+      <c r="T6" s="102"/>
+      <c r="U6" s="102"/>
+      <c r="V6" s="103"/>
       <c r="W6" s="10"/>
     </row>
     <row r="7" spans="1:23" ht="18" x14ac:dyDescent="0.35">
@@ -4143,13 +4143,13 @@
         <v>Done</v>
       </c>
       <c r="Q14" s="8"/>
-      <c r="R14" s="95" t="s">
+      <c r="R14" s="99" t="s">
         <v>44</v>
       </c>
-      <c r="S14" s="98"/>
-      <c r="T14" s="98"/>
-      <c r="U14" s="98"/>
-      <c r="V14" s="99"/>
+      <c r="S14" s="102"/>
+      <c r="T14" s="102"/>
+      <c r="U14" s="102"/>
+      <c r="V14" s="103"/>
       <c r="W14" s="10"/>
     </row>
     <row r="15" spans="1:23" x14ac:dyDescent="0.3">
@@ -4186,10 +4186,10 @@
       </c>
       <c r="Q15" s="44"/>
       <c r="R15" s="70"/>
-      <c r="S15" s="100" t="s">
+      <c r="S15" s="87" t="s">
         <v>33</v>
       </c>
-      <c r="T15" s="100"/>
+      <c r="T15" s="87"/>
       <c r="U15" s="44">
         <f>SUM(E6:E25)</f>
         <v>45.5</v>
@@ -4233,10 +4233,10 @@
       </c>
       <c r="Q16" s="44"/>
       <c r="R16" s="70"/>
-      <c r="S16" s="101" t="s">
+      <c r="S16" s="88" t="s">
         <v>34</v>
       </c>
-      <c r="T16" s="101"/>
+      <c r="T16" s="88"/>
       <c r="U16" s="44">
         <f>SUMIF(F6:O25,"&lt;0")*-1</f>
         <v>42.5</v>
@@ -4273,11 +4273,11 @@
         <v>Done</v>
       </c>
       <c r="Q17" s="44"/>
-      <c r="R17" s="102" t="s">
+      <c r="R17" s="89" t="s">
         <v>35</v>
       </c>
-      <c r="S17" s="103"/>
-      <c r="T17" s="103"/>
+      <c r="S17" s="90"/>
+      <c r="T17" s="90"/>
       <c r="U17" s="75">
         <f>SUM(U15,U16)</f>
         <v>88</v>
@@ -4422,13 +4422,13 @@
         <v>Incomplete</v>
       </c>
       <c r="Q21" s="44"/>
-      <c r="R21" s="95" t="s">
+      <c r="R21" s="99" t="s">
         <v>43</v>
       </c>
-      <c r="S21" s="96"/>
-      <c r="T21" s="96"/>
-      <c r="U21" s="96"/>
-      <c r="V21" s="97"/>
+      <c r="S21" s="100"/>
+      <c r="T21" s="100"/>
+      <c r="U21" s="100"/>
+      <c r="V21" s="101"/>
       <c r="W21" s="10"/>
     </row>
     <row r="22" spans="1:24" x14ac:dyDescent="0.3">
@@ -4461,10 +4461,10 @@
       </c>
       <c r="Q22" s="44"/>
       <c r="R22" s="70"/>
-      <c r="S22" s="100" t="s">
+      <c r="S22" s="87" t="s">
         <v>39</v>
       </c>
-      <c r="T22" s="100"/>
+      <c r="T22" s="87"/>
       <c r="U22" s="44">
         <f>SUMIF(F6:J25,"&gt;0")</f>
         <v>35.5</v>
@@ -4502,10 +4502,10 @@
       </c>
       <c r="Q23" s="44"/>
       <c r="R23" s="70"/>
-      <c r="S23" s="101" t="s">
+      <c r="S23" s="88" t="s">
         <v>38</v>
       </c>
-      <c r="T23" s="101"/>
+      <c r="T23" s="88"/>
       <c r="U23" s="78">
         <f>SUMIF(K6:O25,"&gt;0")</f>
         <v>36</v>
@@ -4546,11 +4546,11 @@
         <v>Incomplete</v>
       </c>
       <c r="Q24" s="44"/>
-      <c r="R24" s="102" t="s">
+      <c r="R24" s="89" t="s">
         <v>37</v>
       </c>
-      <c r="S24" s="103"/>
-      <c r="T24" s="103"/>
+      <c r="S24" s="90"/>
+      <c r="T24" s="90"/>
       <c r="U24" s="77">
         <f>SUM(U22,U23)</f>
         <v>71.5</v>
@@ -5024,12 +5024,6 @@
     </customSheetView>
   </customSheetViews>
   <mergeCells count="13">
-    <mergeCell ref="S22:T22"/>
-    <mergeCell ref="S23:T23"/>
-    <mergeCell ref="R24:T24"/>
-    <mergeCell ref="R17:T17"/>
-    <mergeCell ref="S15:T15"/>
-    <mergeCell ref="S16:T16"/>
     <mergeCell ref="B1:W1"/>
     <mergeCell ref="B2:W2"/>
     <mergeCell ref="F3:J3"/>
@@ -5037,6 +5031,12 @@
     <mergeCell ref="R21:V21"/>
     <mergeCell ref="R6:V6"/>
     <mergeCell ref="R14:V14"/>
+    <mergeCell ref="S22:T22"/>
+    <mergeCell ref="S23:T23"/>
+    <mergeCell ref="R24:T24"/>
+    <mergeCell ref="R17:T17"/>
+    <mergeCell ref="S15:T15"/>
+    <mergeCell ref="S16:T16"/>
   </mergeCells>
   <conditionalFormatting sqref="P6:P25">
     <cfRule type="containsText" dxfId="15" priority="8" operator="containsText" text="Incomplete">
@@ -5136,57 +5136,57 @@
   <sheetData>
     <row r="1" spans="1:23" ht="49.8" x14ac:dyDescent="0.8">
       <c r="A1" s="24"/>
-      <c r="B1" s="87" t="s">
+      <c r="B1" s="91" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="87"/>
-      <c r="D1" s="87"/>
-      <c r="E1" s="87"/>
-      <c r="F1" s="87"/>
-      <c r="G1" s="87"/>
-      <c r="H1" s="87"/>
-      <c r="I1" s="87"/>
-      <c r="J1" s="87"/>
-      <c r="K1" s="87"/>
-      <c r="L1" s="87"/>
-      <c r="M1" s="87"/>
-      <c r="N1" s="87"/>
-      <c r="O1" s="87"/>
-      <c r="P1" s="87"/>
-      <c r="Q1" s="87"/>
-      <c r="R1" s="87"/>
-      <c r="S1" s="87"/>
-      <c r="T1" s="87"/>
-      <c r="U1" s="87"/>
-      <c r="V1" s="87"/>
-      <c r="W1" s="87"/>
+      <c r="C1" s="91"/>
+      <c r="D1" s="91"/>
+      <c r="E1" s="91"/>
+      <c r="F1" s="91"/>
+      <c r="G1" s="91"/>
+      <c r="H1" s="91"/>
+      <c r="I1" s="91"/>
+      <c r="J1" s="91"/>
+      <c r="K1" s="91"/>
+      <c r="L1" s="91"/>
+      <c r="M1" s="91"/>
+      <c r="N1" s="91"/>
+      <c r="O1" s="91"/>
+      <c r="P1" s="91"/>
+      <c r="Q1" s="91"/>
+      <c r="R1" s="91"/>
+      <c r="S1" s="91"/>
+      <c r="T1" s="91"/>
+      <c r="U1" s="91"/>
+      <c r="V1" s="91"/>
+      <c r="W1" s="91"/>
     </row>
     <row r="2" spans="1:23" ht="33" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A2" s="24"/>
-      <c r="B2" s="88" t="s">
+      <c r="B2" s="92" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="88"/>
-      <c r="D2" s="88"/>
-      <c r="E2" s="88"/>
-      <c r="F2" s="88"/>
-      <c r="G2" s="88"/>
-      <c r="H2" s="88"/>
-      <c r="I2" s="88"/>
-      <c r="J2" s="88"/>
-      <c r="K2" s="88"/>
-      <c r="L2" s="88"/>
-      <c r="M2" s="88"/>
-      <c r="N2" s="88"/>
-      <c r="O2" s="88"/>
-      <c r="P2" s="88"/>
-      <c r="Q2" s="88"/>
-      <c r="R2" s="88"/>
-      <c r="S2" s="88"/>
-      <c r="T2" s="88"/>
-      <c r="U2" s="88"/>
-      <c r="V2" s="88"/>
-      <c r="W2" s="88"/>
+      <c r="C2" s="92"/>
+      <c r="D2" s="92"/>
+      <c r="E2" s="92"/>
+      <c r="F2" s="92"/>
+      <c r="G2" s="92"/>
+      <c r="H2" s="92"/>
+      <c r="I2" s="92"/>
+      <c r="J2" s="92"/>
+      <c r="K2" s="92"/>
+      <c r="L2" s="92"/>
+      <c r="M2" s="92"/>
+      <c r="N2" s="92"/>
+      <c r="O2" s="92"/>
+      <c r="P2" s="92"/>
+      <c r="Q2" s="92"/>
+      <c r="R2" s="92"/>
+      <c r="S2" s="92"/>
+      <c r="T2" s="92"/>
+      <c r="U2" s="92"/>
+      <c r="V2" s="92"/>
+      <c r="W2" s="92"/>
     </row>
     <row r="3" spans="1:23" s="1" customFormat="1" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="22"/>
@@ -5194,20 +5194,20 @@
       <c r="C3" s="30"/>
       <c r="D3" s="30"/>
       <c r="E3" s="30"/>
-      <c r="F3" s="89" t="s">
+      <c r="F3" s="93" t="s">
         <v>31</v>
       </c>
-      <c r="G3" s="90"/>
-      <c r="H3" s="90"/>
-      <c r="I3" s="90"/>
-      <c r="J3" s="91"/>
-      <c r="K3" s="92" t="s">
+      <c r="G3" s="94"/>
+      <c r="H3" s="94"/>
+      <c r="I3" s="94"/>
+      <c r="J3" s="95"/>
+      <c r="K3" s="96" t="s">
         <v>32</v>
       </c>
-      <c r="L3" s="93"/>
-      <c r="M3" s="93"/>
-      <c r="N3" s="93"/>
-      <c r="O3" s="94"/>
+      <c r="L3" s="97"/>
+      <c r="M3" s="97"/>
+      <c r="N3" s="97"/>
+      <c r="O3" s="98"/>
       <c r="P3" s="62"/>
       <c r="Q3" s="31"/>
       <c r="R3" s="31"/>
@@ -5345,13 +5345,13 @@
         <f t="shared" ref="P6:P25" si="0">IF(D6="","-",(IF(COUNT(E6:O6) = 0,"To Do",IF(E6&gt;SUM(F6:O6),"Incomplete","Done"))))</f>
         <v>Done</v>
       </c>
-      <c r="R6" s="95" t="s">
+      <c r="R6" s="99" t="s">
         <v>4</v>
       </c>
-      <c r="S6" s="98"/>
-      <c r="T6" s="98"/>
-      <c r="U6" s="98"/>
-      <c r="V6" s="99"/>
+      <c r="S6" s="102"/>
+      <c r="T6" s="102"/>
+      <c r="U6" s="102"/>
+      <c r="V6" s="103"/>
       <c r="W6" s="10"/>
     </row>
     <row r="7" spans="1:23" ht="18" x14ac:dyDescent="0.35">
@@ -5641,13 +5641,13 @@
         <v>Done</v>
       </c>
       <c r="Q14" s="8"/>
-      <c r="R14" s="95" t="s">
+      <c r="R14" s="99" t="s">
         <v>44</v>
       </c>
-      <c r="S14" s="98"/>
-      <c r="T14" s="98"/>
-      <c r="U14" s="98"/>
-      <c r="V14" s="99"/>
+      <c r="S14" s="102"/>
+      <c r="T14" s="102"/>
+      <c r="U14" s="102"/>
+      <c r="V14" s="103"/>
       <c r="W14" s="10"/>
     </row>
     <row r="15" spans="1:23" x14ac:dyDescent="0.3">
@@ -5680,10 +5680,10 @@
       </c>
       <c r="Q15" s="44"/>
       <c r="R15" s="70"/>
-      <c r="S15" s="100" t="s">
+      <c r="S15" s="87" t="s">
         <v>33</v>
       </c>
-      <c r="T15" s="100"/>
+      <c r="T15" s="87"/>
       <c r="U15" s="44">
         <f>SUM(E6:E25)</f>
         <v>48</v>
@@ -5721,10 +5721,10 @@
       </c>
       <c r="Q16" s="44"/>
       <c r="R16" s="70"/>
-      <c r="S16" s="101" t="s">
+      <c r="S16" s="88" t="s">
         <v>34</v>
       </c>
-      <c r="T16" s="101"/>
+      <c r="T16" s="88"/>
       <c r="U16" s="44">
         <f>SUMIF(F6:O25,"&lt;0")*-1</f>
         <v>4</v>
@@ -5755,11 +5755,11 @@
         <v>-</v>
       </c>
       <c r="Q17" s="44"/>
-      <c r="R17" s="102" t="s">
+      <c r="R17" s="89" t="s">
         <v>35</v>
       </c>
-      <c r="S17" s="103"/>
-      <c r="T17" s="103"/>
+      <c r="S17" s="90"/>
+      <c r="T17" s="90"/>
       <c r="U17" s="75">
         <f>SUM(U15,U16)</f>
         <v>52</v>
@@ -5872,13 +5872,13 @@
         <v>-</v>
       </c>
       <c r="Q21" s="44"/>
-      <c r="R21" s="95" t="s">
+      <c r="R21" s="99" t="s">
         <v>43</v>
       </c>
-      <c r="S21" s="96"/>
-      <c r="T21" s="96"/>
-      <c r="U21" s="96"/>
-      <c r="V21" s="97"/>
+      <c r="S21" s="100"/>
+      <c r="T21" s="100"/>
+      <c r="U21" s="100"/>
+      <c r="V21" s="101"/>
       <c r="W21" s="10"/>
     </row>
     <row r="22" spans="1:24" x14ac:dyDescent="0.3">
@@ -5905,10 +5905,10 @@
       </c>
       <c r="Q22" s="44"/>
       <c r="R22" s="70"/>
-      <c r="S22" s="100" t="s">
+      <c r="S22" s="87" t="s">
         <v>39</v>
       </c>
-      <c r="T22" s="100"/>
+      <c r="T22" s="87"/>
       <c r="U22" s="44">
         <f>SUMIF(F6:J25,"&gt;0")</f>
         <v>13.25</v>
@@ -5940,10 +5940,10 @@
       </c>
       <c r="Q23" s="44"/>
       <c r="R23" s="70"/>
-      <c r="S23" s="101" t="s">
+      <c r="S23" s="88" t="s">
         <v>38</v>
       </c>
-      <c r="T23" s="101"/>
+      <c r="T23" s="88"/>
       <c r="U23" s="78">
         <f>SUMIF(K6:O25,"&gt;0")</f>
         <v>38.75</v>
@@ -5974,11 +5974,11 @@
         <v>-</v>
       </c>
       <c r="Q24" s="44"/>
-      <c r="R24" s="102" t="s">
+      <c r="R24" s="89" t="s">
         <v>37</v>
       </c>
-      <c r="S24" s="103"/>
-      <c r="T24" s="103"/>
+      <c r="S24" s="90"/>
+      <c r="T24" s="90"/>
       <c r="U24" s="77">
         <f>SUM(U22,U23)</f>
         <v>52</v>
@@ -6440,6 +6440,12 @@
   </sheetData>
   <autoFilter ref="C4:O27"/>
   <mergeCells count="13">
+    <mergeCell ref="R14:V14"/>
+    <mergeCell ref="B1:W1"/>
+    <mergeCell ref="B2:W2"/>
+    <mergeCell ref="F3:J3"/>
+    <mergeCell ref="K3:O3"/>
+    <mergeCell ref="R6:V6"/>
     <mergeCell ref="R24:T24"/>
     <mergeCell ref="S15:T15"/>
     <mergeCell ref="S16:T16"/>
@@ -6447,12 +6453,6 @@
     <mergeCell ref="R21:V21"/>
     <mergeCell ref="S22:T22"/>
     <mergeCell ref="S23:T23"/>
-    <mergeCell ref="R14:V14"/>
-    <mergeCell ref="B1:W1"/>
-    <mergeCell ref="B2:W2"/>
-    <mergeCell ref="F3:J3"/>
-    <mergeCell ref="K3:O3"/>
-    <mergeCell ref="R6:V6"/>
   </mergeCells>
   <conditionalFormatting sqref="P6:P25">
     <cfRule type="containsText" dxfId="11" priority="3" operator="containsText" text="Incomplete">
@@ -6552,57 +6552,57 @@
   <sheetData>
     <row r="1" spans="1:23" ht="49.8" x14ac:dyDescent="0.8">
       <c r="A1" s="24"/>
-      <c r="B1" s="87" t="s">
+      <c r="B1" s="91" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="87"/>
-      <c r="D1" s="87"/>
-      <c r="E1" s="87"/>
-      <c r="F1" s="87"/>
-      <c r="G1" s="87"/>
-      <c r="H1" s="87"/>
-      <c r="I1" s="87"/>
-      <c r="J1" s="87"/>
-      <c r="K1" s="87"/>
-      <c r="L1" s="87"/>
-      <c r="M1" s="87"/>
-      <c r="N1" s="87"/>
-      <c r="O1" s="87"/>
-      <c r="P1" s="87"/>
-      <c r="Q1" s="87"/>
-      <c r="R1" s="87"/>
-      <c r="S1" s="87"/>
-      <c r="T1" s="87"/>
-      <c r="U1" s="87"/>
-      <c r="V1" s="87"/>
-      <c r="W1" s="87"/>
+      <c r="C1" s="91"/>
+      <c r="D1" s="91"/>
+      <c r="E1" s="91"/>
+      <c r="F1" s="91"/>
+      <c r="G1" s="91"/>
+      <c r="H1" s="91"/>
+      <c r="I1" s="91"/>
+      <c r="J1" s="91"/>
+      <c r="K1" s="91"/>
+      <c r="L1" s="91"/>
+      <c r="M1" s="91"/>
+      <c r="N1" s="91"/>
+      <c r="O1" s="91"/>
+      <c r="P1" s="91"/>
+      <c r="Q1" s="91"/>
+      <c r="R1" s="91"/>
+      <c r="S1" s="91"/>
+      <c r="T1" s="91"/>
+      <c r="U1" s="91"/>
+      <c r="V1" s="91"/>
+      <c r="W1" s="91"/>
     </row>
     <row r="2" spans="1:23" ht="33" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A2" s="24"/>
-      <c r="B2" s="88" t="s">
+      <c r="B2" s="92" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="88"/>
-      <c r="D2" s="88"/>
-      <c r="E2" s="88"/>
-      <c r="F2" s="88"/>
-      <c r="G2" s="88"/>
-      <c r="H2" s="88"/>
-      <c r="I2" s="88"/>
-      <c r="J2" s="88"/>
-      <c r="K2" s="88"/>
-      <c r="L2" s="88"/>
-      <c r="M2" s="88"/>
-      <c r="N2" s="88"/>
-      <c r="O2" s="88"/>
-      <c r="P2" s="88"/>
-      <c r="Q2" s="88"/>
-      <c r="R2" s="88"/>
-      <c r="S2" s="88"/>
-      <c r="T2" s="88"/>
-      <c r="U2" s="88"/>
-      <c r="V2" s="88"/>
-      <c r="W2" s="88"/>
+      <c r="C2" s="92"/>
+      <c r="D2" s="92"/>
+      <c r="E2" s="92"/>
+      <c r="F2" s="92"/>
+      <c r="G2" s="92"/>
+      <c r="H2" s="92"/>
+      <c r="I2" s="92"/>
+      <c r="J2" s="92"/>
+      <c r="K2" s="92"/>
+      <c r="L2" s="92"/>
+      <c r="M2" s="92"/>
+      <c r="N2" s="92"/>
+      <c r="O2" s="92"/>
+      <c r="P2" s="92"/>
+      <c r="Q2" s="92"/>
+      <c r="R2" s="92"/>
+      <c r="S2" s="92"/>
+      <c r="T2" s="92"/>
+      <c r="U2" s="92"/>
+      <c r="V2" s="92"/>
+      <c r="W2" s="92"/>
     </row>
     <row r="3" spans="1:23" s="1" customFormat="1" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="22"/>
@@ -6610,20 +6610,20 @@
       <c r="C3" s="30"/>
       <c r="D3" s="30"/>
       <c r="E3" s="30"/>
-      <c r="F3" s="89" t="s">
+      <c r="F3" s="93" t="s">
         <v>31</v>
       </c>
-      <c r="G3" s="90"/>
-      <c r="H3" s="90"/>
-      <c r="I3" s="90"/>
-      <c r="J3" s="91"/>
-      <c r="K3" s="92" t="s">
+      <c r="G3" s="94"/>
+      <c r="H3" s="94"/>
+      <c r="I3" s="94"/>
+      <c r="J3" s="95"/>
+      <c r="K3" s="96" t="s">
         <v>32</v>
       </c>
-      <c r="L3" s="93"/>
-      <c r="M3" s="93"/>
-      <c r="N3" s="93"/>
-      <c r="O3" s="94"/>
+      <c r="L3" s="97"/>
+      <c r="M3" s="97"/>
+      <c r="N3" s="97"/>
+      <c r="O3" s="98"/>
       <c r="P3" s="62"/>
       <c r="Q3" s="31"/>
       <c r="R3" s="31"/>
@@ -6757,13 +6757,13 @@
         <f t="shared" ref="P6:P25" si="0">IF(D6="","-",(IF(COUNT(E6:O6) = 0,"To Do",IF(E6&gt;SUM(F6:O6),"Incomplete","Done"))))</f>
         <v>Done</v>
       </c>
-      <c r="R6" s="95" t="s">
+      <c r="R6" s="99" t="s">
         <v>4</v>
       </c>
-      <c r="S6" s="98"/>
-      <c r="T6" s="98"/>
-      <c r="U6" s="98"/>
-      <c r="V6" s="99"/>
+      <c r="S6" s="102"/>
+      <c r="T6" s="102"/>
+      <c r="U6" s="102"/>
+      <c r="V6" s="103"/>
       <c r="W6" s="10"/>
     </row>
     <row r="7" spans="1:23" ht="18" x14ac:dyDescent="0.35">
@@ -7045,13 +7045,13 @@
         <v>Done</v>
       </c>
       <c r="Q14" s="8"/>
-      <c r="R14" s="95" t="s">
+      <c r="R14" s="99" t="s">
         <v>44</v>
       </c>
-      <c r="S14" s="98"/>
-      <c r="T14" s="98"/>
-      <c r="U14" s="98"/>
-      <c r="V14" s="99"/>
+      <c r="S14" s="102"/>
+      <c r="T14" s="102"/>
+      <c r="U14" s="102"/>
+      <c r="V14" s="103"/>
       <c r="W14" s="10"/>
     </row>
     <row r="15" spans="1:23" x14ac:dyDescent="0.3">
@@ -7084,10 +7084,10 @@
       </c>
       <c r="Q15" s="44"/>
       <c r="R15" s="70"/>
-      <c r="S15" s="100" t="s">
+      <c r="S15" s="87" t="s">
         <v>33</v>
       </c>
-      <c r="T15" s="100"/>
+      <c r="T15" s="87"/>
       <c r="U15" s="44">
         <f>SUM(E6:E25)</f>
         <v>86.5</v>
@@ -7121,10 +7121,10 @@
       </c>
       <c r="Q16" s="44"/>
       <c r="R16" s="70"/>
-      <c r="S16" s="101" t="s">
+      <c r="S16" s="88" t="s">
         <v>34</v>
       </c>
-      <c r="T16" s="101"/>
+      <c r="T16" s="88"/>
       <c r="U16" s="44">
         <f>SUMIF(F6:O25,"&lt;0")*-1</f>
         <v>0</v>
@@ -7165,11 +7165,11 @@
         <v>Done</v>
       </c>
       <c r="Q17" s="44"/>
-      <c r="R17" s="102" t="s">
+      <c r="R17" s="89" t="s">
         <v>35</v>
       </c>
-      <c r="S17" s="103"/>
-      <c r="T17" s="103"/>
+      <c r="S17" s="90"/>
+      <c r="T17" s="90"/>
       <c r="U17" s="75">
         <f>SUM(U15,U16)</f>
         <v>86.5</v>
@@ -7316,13 +7316,13 @@
         <v>Done</v>
       </c>
       <c r="Q21" s="44"/>
-      <c r="R21" s="95" t="s">
+      <c r="R21" s="99" t="s">
         <v>43</v>
       </c>
-      <c r="S21" s="96"/>
-      <c r="T21" s="96"/>
-      <c r="U21" s="96"/>
-      <c r="V21" s="97"/>
+      <c r="S21" s="100"/>
+      <c r="T21" s="100"/>
+      <c r="U21" s="100"/>
+      <c r="V21" s="101"/>
       <c r="W21" s="10"/>
     </row>
     <row r="22" spans="1:24" x14ac:dyDescent="0.3">
@@ -7351,10 +7351,10 @@
       </c>
       <c r="Q22" s="44"/>
       <c r="R22" s="70"/>
-      <c r="S22" s="100" t="s">
+      <c r="S22" s="87" t="s">
         <v>39</v>
       </c>
-      <c r="T22" s="100"/>
+      <c r="T22" s="87"/>
       <c r="U22" s="44">
         <f>SUMIF(F6:J25,"&gt;0")</f>
         <v>44.5</v>
@@ -7392,10 +7392,10 @@
       </c>
       <c r="Q23" s="44"/>
       <c r="R23" s="70"/>
-      <c r="S23" s="101" t="s">
+      <c r="S23" s="88" t="s">
         <v>38</v>
       </c>
-      <c r="T23" s="101"/>
+      <c r="T23" s="88"/>
       <c r="U23" s="78">
         <f>SUMIF(K6:O25,"&gt;0")</f>
         <v>36.5</v>
@@ -7432,11 +7432,11 @@
         <v>Done</v>
       </c>
       <c r="Q24" s="44"/>
-      <c r="R24" s="102" t="s">
+      <c r="R24" s="89" t="s">
         <v>37</v>
       </c>
-      <c r="S24" s="103"/>
-      <c r="T24" s="103"/>
+      <c r="S24" s="90"/>
+      <c r="T24" s="90"/>
       <c r="U24" s="77">
         <f>SUM(U22,U23)</f>
         <v>81</v>
@@ -7898,12 +7898,6 @@
   </sheetData>
   <autoFilter ref="C4:O27"/>
   <mergeCells count="13">
-    <mergeCell ref="R14:V14"/>
-    <mergeCell ref="B1:W1"/>
-    <mergeCell ref="B2:W2"/>
-    <mergeCell ref="F3:J3"/>
-    <mergeCell ref="K3:O3"/>
-    <mergeCell ref="R6:V6"/>
     <mergeCell ref="R24:T24"/>
     <mergeCell ref="S15:T15"/>
     <mergeCell ref="S16:T16"/>
@@ -7911,6 +7905,12 @@
     <mergeCell ref="R21:V21"/>
     <mergeCell ref="S22:T22"/>
     <mergeCell ref="S23:T23"/>
+    <mergeCell ref="R14:V14"/>
+    <mergeCell ref="B1:W1"/>
+    <mergeCell ref="B2:W2"/>
+    <mergeCell ref="F3:J3"/>
+    <mergeCell ref="K3:O3"/>
+    <mergeCell ref="R6:V6"/>
   </mergeCells>
   <conditionalFormatting sqref="P6:P25">
     <cfRule type="containsText" dxfId="7" priority="3" operator="containsText" text="Incomplete">
@@ -7994,7 +7994,7 @@
   <dimension ref="A1:U42"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="L19" sqref="L19"/>
+      <selection activeCell="L15" sqref="L15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8010,51 +8010,51 @@
   <sheetData>
     <row r="1" spans="1:20" ht="49.8" x14ac:dyDescent="0.8">
       <c r="A1" s="24"/>
-      <c r="B1" s="87" t="s">
+      <c r="B1" s="91" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="87"/>
-      <c r="D1" s="87"/>
-      <c r="E1" s="87"/>
-      <c r="F1" s="87"/>
-      <c r="G1" s="87"/>
-      <c r="H1" s="87"/>
-      <c r="I1" s="87"/>
-      <c r="J1" s="87"/>
-      <c r="K1" s="87"/>
-      <c r="L1" s="87"/>
-      <c r="M1" s="87"/>
-      <c r="N1" s="87"/>
-      <c r="O1" s="87"/>
-      <c r="P1" s="87"/>
-      <c r="Q1" s="87"/>
-      <c r="R1" s="87"/>
-      <c r="S1" s="87"/>
-      <c r="T1" s="87"/>
+      <c r="C1" s="91"/>
+      <c r="D1" s="91"/>
+      <c r="E1" s="91"/>
+      <c r="F1" s="91"/>
+      <c r="G1" s="91"/>
+      <c r="H1" s="91"/>
+      <c r="I1" s="91"/>
+      <c r="J1" s="91"/>
+      <c r="K1" s="91"/>
+      <c r="L1" s="91"/>
+      <c r="M1" s="91"/>
+      <c r="N1" s="91"/>
+      <c r="O1" s="91"/>
+      <c r="P1" s="91"/>
+      <c r="Q1" s="91"/>
+      <c r="R1" s="91"/>
+      <c r="S1" s="91"/>
+      <c r="T1" s="91"/>
     </row>
     <row r="2" spans="1:20" ht="33" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A2" s="24"/>
-      <c r="B2" s="88" t="s">
+      <c r="B2" s="92" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="88"/>
-      <c r="D2" s="88"/>
-      <c r="E2" s="88"/>
-      <c r="F2" s="88"/>
-      <c r="G2" s="88"/>
-      <c r="H2" s="88"/>
-      <c r="I2" s="88"/>
-      <c r="J2" s="88"/>
-      <c r="K2" s="88"/>
-      <c r="L2" s="88"/>
-      <c r="M2" s="88"/>
-      <c r="N2" s="88"/>
-      <c r="O2" s="88"/>
-      <c r="P2" s="88"/>
-      <c r="Q2" s="88"/>
-      <c r="R2" s="88"/>
-      <c r="S2" s="88"/>
-      <c r="T2" s="88"/>
+      <c r="C2" s="92"/>
+      <c r="D2" s="92"/>
+      <c r="E2" s="92"/>
+      <c r="F2" s="92"/>
+      <c r="G2" s="92"/>
+      <c r="H2" s="92"/>
+      <c r="I2" s="92"/>
+      <c r="J2" s="92"/>
+      <c r="K2" s="92"/>
+      <c r="L2" s="92"/>
+      <c r="M2" s="92"/>
+      <c r="N2" s="92"/>
+      <c r="O2" s="92"/>
+      <c r="P2" s="92"/>
+      <c r="Q2" s="92"/>
+      <c r="R2" s="92"/>
+      <c r="S2" s="92"/>
+      <c r="T2" s="92"/>
     </row>
     <row r="3" spans="1:20" s="1" customFormat="1" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="22"/>
@@ -8062,14 +8062,14 @@
       <c r="C3" s="30"/>
       <c r="D3" s="30"/>
       <c r="E3" s="30"/>
-      <c r="F3" s="89" t="s">
+      <c r="F3" s="93" t="s">
         <v>31</v>
       </c>
-      <c r="G3" s="90"/>
-      <c r="H3" s="90"/>
-      <c r="I3" s="90"/>
-      <c r="J3" s="91"/>
-      <c r="K3" s="92" t="s">
+      <c r="G3" s="94"/>
+      <c r="H3" s="94"/>
+      <c r="I3" s="94"/>
+      <c r="J3" s="95"/>
+      <c r="K3" s="96" t="s">
         <v>32</v>
       </c>
       <c r="L3" s="104"/>
@@ -8189,13 +8189,13 @@
         <f t="shared" ref="M6:M25" si="0">IF(D6="","-",(IF(COUNT(E6:L6) = 0,"To Do",IF(E6&gt;SUM(F6:L6),"Incomplete","Done"))))</f>
         <v>Done</v>
       </c>
-      <c r="O6" s="95" t="s">
+      <c r="O6" s="99" t="s">
         <v>4</v>
       </c>
-      <c r="P6" s="98"/>
-      <c r="Q6" s="98"/>
-      <c r="R6" s="98"/>
-      <c r="S6" s="99"/>
+      <c r="P6" s="102"/>
+      <c r="Q6" s="102"/>
+      <c r="R6" s="102"/>
+      <c r="S6" s="103"/>
       <c r="T6" s="10"/>
     </row>
     <row r="7" spans="1:20" ht="18" x14ac:dyDescent="0.35">
@@ -8435,7 +8435,7 @@
         <v>83</v>
       </c>
       <c r="E14" s="3">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="F14" s="3"/>
       <c r="G14" s="48"/>
@@ -8449,19 +8449,21 @@
       <c r="K14" s="48">
         <v>7</v>
       </c>
-      <c r="L14" s="48"/>
+      <c r="L14" s="48">
+        <v>2</v>
+      </c>
       <c r="M14" s="76" t="str">
         <f t="shared" si="0"/>
         <v>Done</v>
       </c>
       <c r="N14" s="8"/>
-      <c r="O14" s="95" t="s">
+      <c r="O14" s="99" t="s">
         <v>44</v>
       </c>
-      <c r="P14" s="98"/>
-      <c r="Q14" s="98"/>
-      <c r="R14" s="98"/>
-      <c r="S14" s="99"/>
+      <c r="P14" s="102"/>
+      <c r="Q14" s="102"/>
+      <c r="R14" s="102"/>
+      <c r="S14" s="103"/>
       <c r="T14" s="10"/>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.3">
@@ -8491,13 +8493,13 @@
       </c>
       <c r="N15" s="44"/>
       <c r="O15" s="70"/>
-      <c r="P15" s="100" t="s">
+      <c r="P15" s="87" t="s">
         <v>33</v>
       </c>
-      <c r="Q15" s="100"/>
+      <c r="Q15" s="87"/>
       <c r="R15" s="44">
         <f>SUM(E6:E25)</f>
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="S15" s="71"/>
       <c r="T15" s="10"/>
@@ -8525,10 +8527,10 @@
       </c>
       <c r="N16" s="44"/>
       <c r="O16" s="70"/>
-      <c r="P16" s="101" t="s">
+      <c r="P16" s="88" t="s">
         <v>34</v>
       </c>
-      <c r="Q16" s="101"/>
+      <c r="Q16" s="88"/>
       <c r="R16" s="44">
         <f>SUMIF(F6:L25,"&lt;0")*-1</f>
         <v>1.5</v>
@@ -8562,14 +8564,14 @@
         <v>Done</v>
       </c>
       <c r="N17" s="44"/>
-      <c r="O17" s="102" t="s">
+      <c r="O17" s="89" t="s">
         <v>35</v>
       </c>
-      <c r="P17" s="103"/>
-      <c r="Q17" s="103"/>
+      <c r="P17" s="90"/>
+      <c r="Q17" s="90"/>
       <c r="R17" s="75">
         <f>SUM(R15,R16)</f>
-        <v>78.5</v>
+        <v>80.5</v>
       </c>
       <c r="S17" s="71"/>
       <c r="T17" s="10"/>
@@ -8673,13 +8675,13 @@
         <v>-</v>
       </c>
       <c r="N21" s="44"/>
-      <c r="O21" s="95" t="s">
+      <c r="O21" s="99" t="s">
         <v>43</v>
       </c>
-      <c r="P21" s="96"/>
-      <c r="Q21" s="96"/>
-      <c r="R21" s="96"/>
-      <c r="S21" s="97"/>
+      <c r="P21" s="100"/>
+      <c r="Q21" s="100"/>
+      <c r="R21" s="100"/>
+      <c r="S21" s="101"/>
       <c r="T21" s="10"/>
     </row>
     <row r="22" spans="1:21" x14ac:dyDescent="0.3">
@@ -8703,10 +8705,10 @@
       </c>
       <c r="N22" s="44"/>
       <c r="O22" s="70"/>
-      <c r="P22" s="100" t="s">
+      <c r="P22" s="87" t="s">
         <v>39</v>
       </c>
-      <c r="Q22" s="100"/>
+      <c r="Q22" s="87"/>
       <c r="R22" s="44">
         <f>SUMIF(F6:J25,"&gt;0")</f>
         <v>60</v>
@@ -8743,13 +8745,13 @@
       </c>
       <c r="N23" s="44"/>
       <c r="O23" s="70"/>
-      <c r="P23" s="101" t="s">
+      <c r="P23" s="88" t="s">
         <v>38</v>
       </c>
-      <c r="Q23" s="101"/>
+      <c r="Q23" s="88"/>
       <c r="R23" s="78">
         <f>SUMIF(K6:L25,"&gt;0")</f>
-        <v>18.5</v>
+        <v>20.5</v>
       </c>
       <c r="S23" s="71"/>
       <c r="T23" s="10"/>
@@ -8780,14 +8782,14 @@
         <v>Done</v>
       </c>
       <c r="N24" s="44"/>
-      <c r="O24" s="102" t="s">
+      <c r="O24" s="89" t="s">
         <v>37</v>
       </c>
-      <c r="P24" s="103"/>
-      <c r="Q24" s="103"/>
+      <c r="P24" s="90"/>
+      <c r="Q24" s="90"/>
       <c r="R24" s="77">
         <f>SUM(R22,R23)</f>
-        <v>78.5</v>
+        <v>80.5</v>
       </c>
       <c r="S24" s="71"/>
       <c r="T24" s="10"/>
@@ -8848,31 +8850,31 @@
       </c>
       <c r="E26" s="68">
         <f>SUM(E6:E25)</f>
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="F26" s="50">
         <f>E26-SUM(F6:F25)</f>
-        <v>65.5</v>
+        <v>67.5</v>
       </c>
       <c r="G26" s="50">
         <f>F26-SUM(G6:G25)</f>
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="H26" s="50">
         <f t="shared" ref="H26:L26" si="1">G26-SUM(H6:H25)</f>
-        <v>42.5</v>
+        <v>44.5</v>
       </c>
       <c r="I26" s="50">
         <f t="shared" si="1"/>
-        <v>25.5</v>
+        <v>27.5</v>
       </c>
       <c r="J26" s="50">
         <f t="shared" si="1"/>
-        <v>18.5</v>
+        <v>20.5</v>
       </c>
       <c r="K26" s="50">
         <f t="shared" si="1"/>
-        <v>1.5</v>
+        <v>3.5</v>
       </c>
       <c r="L26" s="50">
         <f t="shared" si="1"/>
@@ -8896,31 +8898,31 @@
       </c>
       <c r="E27" s="38">
         <f>E26</f>
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="F27" s="40">
         <f t="shared" ref="F27:L27" si="2">E27-($E$26/7)</f>
-        <v>66</v>
+        <v>67.714285714285708</v>
       </c>
       <c r="G27" s="40">
         <f t="shared" si="2"/>
-        <v>55</v>
+        <v>56.428571428571423</v>
       </c>
       <c r="H27" s="40">
         <f t="shared" si="2"/>
-        <v>44</v>
+        <v>45.142857142857139</v>
       </c>
       <c r="I27" s="40">
         <f t="shared" si="2"/>
-        <v>33</v>
+        <v>33.857142857142854</v>
       </c>
       <c r="J27" s="40">
         <f t="shared" si="2"/>
-        <v>22</v>
+        <v>22.571428571428569</v>
       </c>
       <c r="K27" s="40">
         <f t="shared" si="2"/>
-        <v>11</v>
+        <v>11.285714285714283</v>
       </c>
       <c r="L27" s="40">
         <f t="shared" si="2"/>
@@ -9183,12 +9185,6 @@
   </sheetData>
   <autoFilter ref="C4:L27"/>
   <mergeCells count="13">
-    <mergeCell ref="O14:S14"/>
-    <mergeCell ref="B1:T1"/>
-    <mergeCell ref="B2:T2"/>
-    <mergeCell ref="F3:J3"/>
-    <mergeCell ref="K3:L3"/>
-    <mergeCell ref="O6:S6"/>
     <mergeCell ref="O24:Q24"/>
     <mergeCell ref="P15:Q15"/>
     <mergeCell ref="P16:Q16"/>
@@ -9196,6 +9192,12 @@
     <mergeCell ref="O21:S21"/>
     <mergeCell ref="P22:Q22"/>
     <mergeCell ref="P23:Q23"/>
+    <mergeCell ref="O14:S14"/>
+    <mergeCell ref="B1:T1"/>
+    <mergeCell ref="B2:T2"/>
+    <mergeCell ref="F3:J3"/>
+    <mergeCell ref="K3:L3"/>
+    <mergeCell ref="O6:S6"/>
   </mergeCells>
   <conditionalFormatting sqref="M6:M25">
     <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="Incomplete">

</xml_diff>